<commit_message>
submission obj & reb
</commit_message>
<xml_diff>
--- a/ADCVD_OBJECTS_STATUS_VALIDATION/input_data/datapool/adcvd_status_validation.xlsx
+++ b/ADCVD_OBJECTS_STATUS_VALIDATION/input_data/datapool/adcvd_status_validation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37451212-0542-4EAD-9FE5-8081FDC25807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66937AEF-AF06-482D-80FE-390316D6C2AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="472" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -872,7 +872,7 @@
         <v>14</v>
       </c>
       <c r="J4" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -904,7 +904,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -936,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -968,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="J7" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1000,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="J8" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1032,7 +1032,7 @@
         <v>14</v>
       </c>
       <c r="J9" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1064,7 +1064,7 @@
         <v>14</v>
       </c>
       <c r="J10" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1096,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="J11" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1128,7 +1128,7 @@
         <v>14</v>
       </c>
       <c r="J12" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>